<commit_message>
updated example excel input sheet naming
</commit_message>
<xml_diff>
--- a/input/_excel/example.xlsx
+++ b/input/_excel/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga35vuk\Desktop\mg_ev_opti\input\_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2F1CD8-5FD7-4C55-8BD4-7CA602E5A151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F51271-37BB-4D93-901C-EE7D41CB4E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{77293274-C4CB-421E-9B2C-ED6957626F24}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="0_mg_go" sheetId="1" r:id="rId2"/>
     <sheet name="1_mgev_go" sheetId="4" r:id="rId3"/>
     <sheet name="2_mg_rh" sheetId="5" r:id="rId4"/>
-    <sheet name="2_mgev_rh" sheetId="6" r:id="rId5"/>
+    <sheet name="3_mgev_rh" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>

<commit_message>
Improved economic result calculation for CommoditySystems, added CommoditySystem Power to plotting, integrated grid resource, displaying NPC and LCOE after run
</commit_message>
<xml_diff>
--- a/input/_excel/example.xlsx
+++ b/input/_excel/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga35vuk\Desktop\mg_ev_opti\input\_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE623A83-ED8D-4930-BB6E-0636D9F92DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F951A2-9825-4856-A76D-D2C9A71F65B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{77293274-C4CB-421E-9B2C-ED6957626F24}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="4" xr2:uid="{77293274-C4CB-421E-9B2C-ED6957626F24}"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1579" uniqueCount="241">
   <si>
     <t>General Simulation</t>
   </si>
@@ -733,13 +733,43 @@
   </si>
   <si>
     <t>go</t>
+  </si>
+  <si>
+    <t>core_opt</t>
+  </si>
+  <si>
+    <t>core_cs</t>
+  </si>
+  <si>
+    <t>core_sce</t>
+  </si>
+  <si>
+    <t>core_eff</t>
+  </si>
+  <si>
+    <t>unitless conversion efficiency of both (ac_dc and dc_ac) bus transformer components</t>
+  </si>
+  <si>
+    <t>core_sme</t>
+  </si>
+  <si>
+    <t>core_soe</t>
+  </si>
+  <si>
+    <t>core_ls</t>
+  </si>
+  <si>
+    <t>core_cdc</t>
+  </si>
+  <si>
+    <t>nominal component size, only used if core_opt is "False"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -822,6 +852,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -861,7 +903,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -917,6 +959,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6656,10 +6708,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A23578-0AE8-47E7-9F24-20E3F0FA7C34}">
-  <dimension ref="A1:E136"/>
+  <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -6823,711 +6875,696 @@
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="5">
-        <v>0.95</v>
+      <c r="A16" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="5">
-        <v>0.95</v>
+        <v>232</v>
+      </c>
+      <c r="B17" s="16">
+        <v>10000000</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>31</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="B18" s="11">
+      <c r="A18" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="B18" s="25">
         <v>0.08</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="27" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
+    <row r="19" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B19" s="5">
+        <f>0.03*B18</f>
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>224</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>225</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="21" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>34</v>
+        <v>238</v>
+      </c>
+      <c r="B21" s="5">
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="14"/>
+      <c r="A22" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="23" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>42</v>
+        <v>234</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0.95</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>36</v>
-      </c>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
         <v>35</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="16">
-        <v>100000</v>
-      </c>
-      <c r="C28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="A28" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="14"/>
     </row>
     <row r="29" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="5">
-        <v>2.8</v>
-      </c>
-      <c r="C31" t="s">
-        <v>223</v>
-      </c>
+      <c r="A29" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="5">
-        <f>0.03*B31</f>
-        <v>8.3999999999999991E-2</v>
+        <v>45</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>224</v>
+        <v>35</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="5">
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>225</v>
+        <v>35</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="5">
-        <v>20</v>
+      <c r="A34" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="16">
+        <v>100000</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35" s="5">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="5"/>
-    </row>
-    <row r="37" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="2"/>
+      <c r="A35" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="5">
+        <v>2.8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="38" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>34</v>
+        <v>58</v>
+      </c>
+      <c r="B38" s="5">
+        <f>0.03*B37</f>
+        <v>8.3999999999999991E-2</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>224</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>46</v>
+        <v>60</v>
+      </c>
+      <c r="B39" s="5">
+        <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>35</v>
+        <v>225</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B40" s="16">
-        <v>750000</v>
+        <v>62</v>
+      </c>
+      <c r="B40" s="5">
+        <v>20</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B43" s="5">
-        <v>11</v>
-      </c>
-      <c r="C43" t="s">
-        <v>76</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>77</v>
-      </c>
+      <c r="A41" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="5">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="5"/>
+    </row>
+    <row r="43" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" s="5">
-        <v>0</v>
+        <v>67</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>79</v>
+        <v>35</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>3</v>
+        <v>46</v>
+      </c>
+      <c r="C45" t="s">
+        <v>35</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B46" s="5">
-        <v>0.503</v>
+        <v>69</v>
+      </c>
+      <c r="B46" s="16">
+        <v>750000</v>
       </c>
       <c r="C46" t="s">
-        <v>226</v>
+        <v>50</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47" s="5">
-        <f>0.03*B46</f>
-        <v>1.5089999999999999E-2</v>
-      </c>
-      <c r="C47" t="s">
-        <v>227</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>59</v>
+      <c r="A47" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="5">
-        <v>0</v>
-      </c>
-      <c r="C48" t="s">
-        <v>225</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>61</v>
+        <v>73</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B49" s="5">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>63</v>
+        <v>76</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B50" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>88</v>
+        <v>76</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B51" s="5">
-        <v>0.95</v>
+        <v>80</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B52" s="5"/>
-    </row>
-    <row r="53" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="2"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" s="5">
+        <v>0.503</v>
+      </c>
+      <c r="C52" t="s">
+        <v>226</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="5">
+        <f>0.03*B52</f>
+        <v>1.5089999999999999E-2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>227</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="54" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>34</v>
+        <v>85</v>
+      </c>
+      <c r="B54" s="5">
+        <v>0</v>
       </c>
       <c r="C54" t="s">
-        <v>35</v>
+        <v>225</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>46</v>
+        <v>86</v>
+      </c>
+      <c r="B55" s="5">
+        <v>25</v>
       </c>
       <c r="C55" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B56" s="16">
-        <v>50000</v>
+        <v>87</v>
+      </c>
+      <c r="B56" s="5">
+        <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D57" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B58" s="5">
-        <v>0.26100000000000001</v>
-      </c>
-      <c r="C58" t="s">
-        <v>223</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B59" s="5">
-        <f>0.08*B58</f>
-        <v>2.0880000000000003E-2</v>
-      </c>
-      <c r="C59" t="s">
-        <v>224</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>59</v>
-      </c>
+      <c r="A57" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B58" s="5"/>
+    </row>
+    <row r="59" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="2"/>
     </row>
     <row r="60" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B60" s="5">
-        <v>6.4999999999999997E-4</v>
+        <v>92</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C60" t="s">
-        <v>225</v>
+        <v>35</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B61" s="5">
-        <v>10</v>
+        <v>93</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="C61" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>101</v>
+        <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B62" s="5">
-        <v>1</v>
+        <v>94</v>
+      </c>
+      <c r="B62" s="16">
+        <v>50000</v>
       </c>
       <c r="C62" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B63" s="11">
-        <v>1</v>
+        <v>96</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D63" s="13" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="18"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="13"/>
-    </row>
-    <row r="65" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="2"/>
+      <c r="A64" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B64" s="5">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="C64" t="s">
+        <v>223</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B65" s="5">
+        <f>0.08*B64</f>
+        <v>2.0880000000000003E-2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>224</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="66" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D66" s="13" t="s">
-        <v>40</v>
+      <c r="A66" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B66" s="5">
+        <v>6.4999999999999997E-4</v>
+      </c>
+      <c r="C66" t="s">
+        <v>225</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B67" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C67" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D67" s="13" t="s">
-        <v>40</v>
+      <c r="A67" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B67" s="5">
+        <v>10</v>
+      </c>
+      <c r="C67" t="s">
+        <v>23</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B68" s="19">
-        <v>30000</v>
-      </c>
-      <c r="C68" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D68" s="13" t="s">
-        <v>40</v>
+      <c r="A68" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B68" s="5">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>3</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A69" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>38</v>
+        <v>103</v>
+      </c>
+      <c r="B69" s="11">
+        <v>1</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="D69" s="13" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="70" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="B70" s="11">
-        <v>15</v>
-      </c>
-      <c r="C70" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="D70" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B71" s="11">
-        <v>0</v>
-      </c>
-      <c r="C71" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="D71" s="13" t="s">
-        <v>40</v>
-      </c>
+      <c r="A70" s="18"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="13"/>
+    </row>
+    <row r="71" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="B72" s="11">
-        <v>3.0000000000000001E-5</v>
+        <v>105</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>225</v>
+        <v>35</v>
       </c>
       <c r="D72" s="13" t="s">
         <v>40</v>
@@ -7535,13 +7572,13 @@
     </row>
     <row r="73" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A73" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B73" s="11">
-        <v>10</v>
+        <v>106</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D73" s="13" t="s">
         <v>40</v>
@@ -7549,13 +7586,13 @@
     </row>
     <row r="74" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B74" s="11">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="B74" s="19">
+        <v>30000</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="D74" s="13" t="s">
         <v>40</v>
@@ -7563,842 +7600,926 @@
     </row>
     <row r="75" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B75" s="11">
-        <v>1</v>
+        <v>108</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D75" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    <row r="76" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B76" s="11">
+        <v>15</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="D76" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B77" s="11">
+        <v>0</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="D77" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B78" s="11">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="D78" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B79" s="11">
+        <v>10</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B80" s="11">
+        <v>1</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D80" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B81" s="11">
+        <v>1</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D81" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C78" t="s">
-        <v>35</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C79" t="s">
-        <v>35</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B80" s="16">
-        <v>1100000</v>
-      </c>
-      <c r="C80" t="s">
-        <v>119</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C81" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D81" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B82" s="5">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="C82" t="s">
-        <v>225</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="B83" s="11">
-        <v>0.14199999999999999</v>
-      </c>
-      <c r="C83" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="D83" s="13" t="s">
-        <v>57</v>
-      </c>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B84" s="5">
-        <f>0.03*B82</f>
-        <v>4.1700000000000001E-3</v>
+        <v>116</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C84" t="s">
-        <v>228</v>
+        <v>35</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
     </row>
     <row r="85" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B85" s="5">
-        <v>0</v>
+        <v>117</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="C85" t="s">
-        <v>225</v>
+        <v>35</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="86" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B86" s="5">
-        <v>10</v>
+        <v>118</v>
+      </c>
+      <c r="B86" s="16">
+        <v>1100000</v>
       </c>
       <c r="C86" t="s">
-        <v>23</v>
+        <v>119</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B87" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="C87" t="s">
-        <v>3</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>127</v>
+        <v>121</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C87" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D87" s="21" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="88" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B88" s="5">
-        <v>0.9</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="C88" t="s">
-        <v>3</v>
+        <v>225</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
     </row>
     <row r="89" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B89" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="C89" t="s">
-        <v>131</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>132</v>
+      <c r="A89" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="B89" s="11">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="D89" s="13" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="90" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B90" s="5">
-        <v>0.8</v>
+        <f>0.03*B88</f>
+        <v>4.1700000000000001E-3</v>
       </c>
       <c r="C90" t="s">
-        <v>131</v>
+        <v>228</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>134</v>
+        <v>59</v>
       </c>
     </row>
     <row r="91" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B91" s="5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C91" t="s">
-        <v>3</v>
+        <v>225</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>136</v>
+        <v>61</v>
       </c>
     </row>
     <row r="92" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B92" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C92" t="s">
-        <v>131</v>
+        <v>23</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>138</v>
+        <v>63</v>
       </c>
     </row>
     <row r="93" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B93" s="5">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C93" t="s">
         <v>3</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
     </row>
     <row r="94" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B94" s="5">
-        <v>1</v>
-      </c>
-      <c r="C94" s="7" t="s">
+        <v>0.9</v>
+      </c>
+      <c r="C94" t="s">
         <v>3</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B95" s="5"/>
-    </row>
-    <row r="96" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="2"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B95" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="C95" t="s">
+        <v>131</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B96" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="C96" t="s">
+        <v>131</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="97" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>34</v>
+        <v>135</v>
+      </c>
+      <c r="B97" s="5">
+        <v>0.5</v>
       </c>
       <c r="C97" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>36</v>
+        <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>46</v>
+        <v>137</v>
+      </c>
+      <c r="B98" s="5">
+        <v>0</v>
       </c>
       <c r="C98" t="s">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
     </row>
     <row r="99" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B99" s="16">
-        <v>30000</v>
+        <v>139</v>
+      </c>
+      <c r="B99" s="5">
+        <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>119</v>
+        <v>3</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>145</v>
+        <v>65</v>
       </c>
     </row>
     <row r="100" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B100" t="s">
-        <v>147</v>
-      </c>
-      <c r="C100" t="s">
-        <v>148</v>
+        <v>140</v>
+      </c>
+      <c r="B100" s="5">
+        <v>1</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="B101" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C101" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D101" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C102" t="s">
-        <v>3</v>
-      </c>
-      <c r="D102" s="6" t="s">
-        <v>153</v>
-      </c>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B101" s="5"/>
+    </row>
+    <row r="102" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="2"/>
     </row>
     <row r="103" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="B103" s="11">
-        <v>0</v>
-      </c>
-      <c r="C103" s="14" t="s">
+      <c r="A103" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C103" t="s">
         <v>35</v>
       </c>
-      <c r="D103" s="13" t="s">
-        <v>155</v>
+      <c r="D103" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="104" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="B104" s="5">
-        <v>5</v>
+        <v>143</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="C104" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>157</v>
+        <v>48</v>
       </c>
     </row>
     <row r="105" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B105" s="5">
-        <v>0.25</v>
+        <v>144</v>
+      </c>
+      <c r="B105" s="16">
+        <v>30000</v>
       </c>
       <c r="C105" t="s">
-        <v>225</v>
+        <v>119</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
     </row>
     <row r="106" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B106" s="5">
-        <f>0.03*B105</f>
-        <v>7.4999999999999997E-3</v>
+        <v>146</v>
+      </c>
+      <c r="B106" t="s">
+        <v>147</v>
       </c>
       <c r="C106" t="s">
-        <v>228</v>
+        <v>148</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>59</v>
+        <v>149</v>
       </c>
     </row>
     <row r="107" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B107" s="5">
-        <v>0</v>
-      </c>
-      <c r="C107" t="s">
-        <v>225</v>
-      </c>
-      <c r="D107" s="6" t="s">
-        <v>61</v>
+      <c r="A107" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B107" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D107" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="108" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B108" s="5">
-        <v>10</v>
+        <v>151</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="C108" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>63</v>
+        <v>153</v>
       </c>
     </row>
     <row r="109" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="B109" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="C109" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D109" s="6" t="s">
-        <v>136</v>
+      <c r="A109" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B109" s="11">
+        <v>0</v>
+      </c>
+      <c r="C109" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D109" s="13" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="110" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B110" s="5">
-        <v>11000</v>
+        <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="111" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B111" s="5">
-        <v>11000</v>
+        <v>0.25</v>
       </c>
       <c r="C111" t="s">
-        <v>50</v>
+        <v>225</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>166</v>
+        <v>57</v>
       </c>
     </row>
     <row r="112" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B112" s="5">
-        <v>1</v>
-      </c>
-      <c r="C112" s="7" t="s">
-        <v>3</v>
+        <f>0.03*B111</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="C112" t="s">
+        <v>228</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>168</v>
+        <v>59</v>
       </c>
     </row>
     <row r="113" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B113" s="5">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="C113" t="s">
-        <v>3</v>
+        <v>225</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>170</v>
+        <v>61</v>
       </c>
     </row>
     <row r="114" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B114" s="5">
-        <v>0.95</v>
+        <v>10</v>
       </c>
       <c r="C114" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>172</v>
+        <v>63</v>
       </c>
     </row>
     <row r="115" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B115" s="5">
-        <v>1</v>
-      </c>
-      <c r="C115" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="C115" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="2"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B116" s="5">
+        <v>11000</v>
+      </c>
+      <c r="C116" t="s">
+        <v>50</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B117" s="5">
+        <v>11000</v>
+      </c>
+      <c r="C117" t="s">
+        <v>50</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="118" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="B118" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C118" t="s">
-        <v>35</v>
+        <v>167</v>
+      </c>
+      <c r="B118" s="5">
+        <v>1</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>36</v>
+        <v>168</v>
       </c>
     </row>
     <row r="119" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>46</v>
+        <v>169</v>
+      </c>
+      <c r="B119" s="5">
+        <v>0.95</v>
       </c>
       <c r="C119" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>48</v>
+        <v>170</v>
       </c>
     </row>
     <row r="120" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B120" s="16">
-        <v>30000</v>
+        <v>171</v>
+      </c>
+      <c r="B120" s="5">
+        <v>0.95</v>
       </c>
       <c r="C120" t="s">
-        <v>119</v>
+        <v>3</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="121" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="B121" t="s">
-        <v>147</v>
+        <v>173</v>
+      </c>
+      <c r="B121" s="5">
+        <v>1</v>
       </c>
       <c r="C121" t="s">
-        <v>148</v>
+        <v>3</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="B122" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C122" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D122" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C123" t="s">
-        <v>3</v>
-      </c>
-      <c r="D123" s="6" t="s">
-        <v>183</v>
-      </c>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B123" s="1"/>
+      <c r="C123" s="1"/>
+      <c r="D123" s="2"/>
     </row>
     <row r="124" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="B124" s="11">
-        <v>0</v>
-      </c>
-      <c r="C124" s="14" t="s">
+      <c r="A124" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C124" t="s">
         <v>35</v>
       </c>
-      <c r="D124" s="13" t="s">
-        <v>155</v>
+      <c r="D124" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="125" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="B125" s="5">
-        <v>10</v>
+        <v>176</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="C125" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>157</v>
+        <v>48</v>
       </c>
     </row>
     <row r="126" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="B126" s="5">
-        <v>0.5</v>
+        <v>177</v>
+      </c>
+      <c r="B126" s="16">
+        <v>30000</v>
       </c>
       <c r="C126" t="s">
-        <v>225</v>
+        <v>119</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>57</v>
+        <v>178</v>
       </c>
     </row>
     <row r="127" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A127" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="B127" s="5">
-        <f>0.03*B126</f>
-        <v>1.4999999999999999E-2</v>
+        <v>179</v>
+      </c>
+      <c r="B127" t="s">
+        <v>147</v>
       </c>
       <c r="C127" t="s">
-        <v>228</v>
+        <v>148</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>59</v>
+        <v>145</v>
       </c>
     </row>
     <row r="128" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B128" s="5">
-        <v>0</v>
-      </c>
-      <c r="C128" t="s">
-        <v>225</v>
-      </c>
-      <c r="D128" s="6" t="s">
-        <v>61</v>
+      <c r="A128" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C128" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D128" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="129" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A129" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="B129" s="5">
-        <v>10</v>
+        <v>181</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>182</v>
       </c>
       <c r="C129" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>63</v>
+        <v>183</v>
       </c>
     </row>
     <row r="130" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B130" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="C130" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D130" s="6" t="s">
-        <v>136</v>
+      <c r="A130" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B130" s="11">
+        <v>0</v>
+      </c>
+      <c r="C130" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D130" s="13" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="131" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A131" s="4" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B131" s="5">
-        <v>3600</v>
+        <v>10</v>
       </c>
       <c r="C131" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
     </row>
     <row r="132" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B132" s="5">
-        <v>3600</v>
+        <v>0.5</v>
       </c>
       <c r="C132" t="s">
-        <v>50</v>
+        <v>225</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>194</v>
+        <v>57</v>
       </c>
     </row>
     <row r="133" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A133" s="4" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B133" s="5">
-        <v>1</v>
-      </c>
-      <c r="C133" s="7" t="s">
-        <v>3</v>
+        <f>0.03*B132</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C133" t="s">
+        <v>228</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>168</v>
+        <v>59</v>
       </c>
     </row>
     <row r="134" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B134" s="5">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="C134" t="s">
-        <v>3</v>
+        <v>225</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>170</v>
+        <v>61</v>
       </c>
     </row>
     <row r="135" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A135" s="4" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B135" s="5">
-        <v>0.95</v>
+        <v>10</v>
       </c>
       <c r="C135" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>172</v>
+        <v>63</v>
       </c>
     </row>
     <row r="136" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B136" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D136" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B137" s="5">
+        <v>3600</v>
+      </c>
+      <c r="C137" t="s">
+        <v>50</v>
+      </c>
+      <c r="D137" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B138" s="5">
+        <v>3600</v>
+      </c>
+      <c r="C138" t="s">
+        <v>50</v>
+      </c>
+      <c r="D138" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B139" s="5">
+        <v>1</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D139" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B140" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="C140" t="s">
+        <v>3</v>
+      </c>
+      <c r="D140" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B141" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="C141" t="s">
+        <v>3</v>
+      </c>
+      <c r="D141" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="B136" s="5">
+      <c r="B142" s="5">
         <v>1</v>
       </c>
-      <c r="C136" t="s">
-        <v>3</v>
-      </c>
-      <c r="D136" s="6" t="s">
+      <c r="C142" t="s">
+        <v>3</v>
+      </c>
+      <c r="D142" s="6" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B100" xr:uid="{12AE0ECF-FF2E-4B4C-A168-7102D5C325A1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B106" xr:uid="{12AE0ECF-FF2E-4B4C-A168-7102D5C325A1}">
       <formula1>"uc,tc,cc,v2v,v2g"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B57 B81 B101 B122 B69" xr:uid="{468A5423-0B4D-48A4-B886-EA9D807709C1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63 B87 B107 B128 B75" xr:uid="{468A5423-0B4D-48A4-B886-EA9D807709C1}">
       <formula1>"AC,DC,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42" xr:uid="{C44B1A35-E19F-46FF-B711-4C0DB641BAF7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48" xr:uid="{C44B1A35-E19F-46FF-B711-4C0DB641BAF7}">
       <formula1>"True, False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22 B29 B41" xr:uid="{F3A79F41-C828-42FD-AFDA-9AF9E8D3D7C3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28 B35 B47" xr:uid="{F3A79F41-C828-42FD-AFDA-9AF9E8D3D7C3}">
       <formula1>"AC, DC"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{9BC52C00-7EC3-4E93-872A-4F4CDEC8A952}">
       <formula1>"go, rh"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B124 B26 B103" xr:uid="{5147E92F-FA9F-4B5C-8DD4-01869E92E7CC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B130 B32 B109" xr:uid="{5147E92F-FA9F-4B5C-8DD4-01869E92E7CC}">
       <formula1>"False, True,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54:B55 B66:B67 B78:B79 B38:B39 B121 B97:B98 B118:B119" xr:uid="{2B4218CC-58F4-421F-8760-FD9A030FA149}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60:B61 B72:B73 B84:B85 B44:B45 B127 B103:B104 B124:B125" xr:uid="{2B4218CC-58F4-421F-8760-FD9A030FA149}">
       <formula1>"True, False,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21 B27:B28" xr:uid="{1947198E-9E60-4D99-B51D-72329A85BDC5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27 B33:B34 B16" xr:uid="{1947198E-9E60-4D99-B51D-72329A85BDC5}">
       <formula1>"False, True"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Included CommoditySystem energy pricing as means of representing sale/rebuy of energy to such a system
</commit_message>
<xml_diff>
--- a/input/_excel/example.xlsx
+++ b/input/_excel/example.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2457" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2529" uniqueCount="246">
   <si>
     <t xml:space="preserve">Global Simulation Options</t>
   </si>
@@ -628,6 +628,18 @@
     <t xml:space="preserve">bev_soe</t>
   </si>
   <si>
+    <t xml:space="preserve">bev_sys_chg_soe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost of energy transferred between main buses and commodity bus (equals revenue through sale of energy to commodity operator -&gt; value has to be negative)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bev_sys_dis_soe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost of energy transferred between commodity bus and system core (equals cost of buying energy back from commodity operator -&gt; value has to be positive)</t>
+  </si>
+  <si>
     <t xml:space="preserve">bev_ls</t>
   </si>
   <si>
@@ -710,6 +722,12 @@
   </si>
   <si>
     <t xml:space="preserve">brs_soe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brs_sys_chg_soe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brs_sys_dis_soe</t>
   </si>
   <si>
     <t xml:space="preserve">brs_ls</t>
@@ -1108,7 +1126,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -1289,10 +1307,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E143"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A111" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A139" activeCellId="0" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -2725,55 +2743,55 @@
         <v>200</v>
       </c>
       <c r="B115" s="11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>69</v>
+        <v>201</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B116" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A117" s="10" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B117" s="11" t="n">
-        <v>11000</v>
+        <v>10</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>203</v>
+        <v>69</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B118" s="11" t="n">
-        <v>11000</v>
-      </c>
-      <c r="C118" s="0" t="s">
-        <v>56</v>
+        <v>0.5</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -2781,10 +2799,10 @@
         <v>206</v>
       </c>
       <c r="B119" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>28</v>
+        <v>11000</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D119" s="12" t="s">
         <v>207</v>
@@ -2795,10 +2813,10 @@
         <v>208</v>
       </c>
       <c r="B120" s="11" t="n">
-        <v>0.95</v>
+        <v>11000</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D120" s="12" t="s">
         <v>209</v>
@@ -2809,9 +2827,9 @@
         <v>210</v>
       </c>
       <c r="B121" s="11" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C121" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D121" s="12" t="s">
@@ -2823,232 +2841,232 @@
         <v>212</v>
       </c>
       <c r="B122" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D122" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A123" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B123" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D123" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A124" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B124" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C122" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D122" s="12" t="s">
+      <c r="C124" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D124" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="124" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="3"/>
-    </row>
-    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A125" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B125" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C125" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D125" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A126" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B126" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C126" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D126" s="12" t="s">
-        <v>87</v>
-      </c>
+    <row r="126" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
+      <c r="D126" s="3"/>
     </row>
     <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B127" s="8" t="n">
-        <v>30000</v>
+        <v>218</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>156</v>
+        <v>54</v>
       </c>
       <c r="D127" s="12" t="s">
-        <v>217</v>
+        <v>76</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>186</v>
+        <v>219</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
       <c r="D128" s="12" t="s">
-        <v>184</v>
+        <v>87</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A129" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="B129" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C129" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D129" s="21" t="s">
-        <v>80</v>
+      <c r="A129" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B129" s="8" t="n">
+        <v>30000</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D129" s="12" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A130" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="B130" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>186</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>28</v>
+        <v>187</v>
       </c>
       <c r="D130" s="12" t="s">
-        <v>222</v>
+        <v>184</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A131" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="B131" s="19" t="n">
-        <v>0</v>
+      <c r="B131" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="D131" s="21" t="s">
-        <v>194</v>
+        <v>80</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A132" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="B132" s="11" t="n">
-        <v>10</v>
+      <c r="B132" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="C132" s="0" t="s">
         <v>28</v>
       </c>
       <c r="D132" s="12" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A133" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="B133" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C133" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D133" s="12" t="s">
-        <v>61</v>
+      <c r="A133" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B133" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C133" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D133" s="21" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A134" s="10" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B134" s="11" t="n">
-        <f aca="false">0.03*B133</f>
-        <v>0.015</v>
+        <v>10</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>162</v>
+        <v>28</v>
       </c>
       <c r="D134" s="12" t="s">
-        <v>64</v>
+        <v>196</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A135" s="10" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B135" s="11" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C135" s="0" t="s">
         <v>66</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A136" s="10" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B136" s="11" t="n">
-        <v>10</v>
+        <f aca="false">0.03*B135</f>
+        <v>0.015</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>48</v>
+        <v>162</v>
       </c>
       <c r="D136" s="12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A137" s="10" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B137" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C137" s="6" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="C137" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="D137" s="12" t="s">
-        <v>175</v>
+        <v>67</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A138" s="10" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B138" s="11" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D138" s="12" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A139" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B139" s="11" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D139" s="12" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -3056,13 +3074,13 @@
         <v>234</v>
       </c>
       <c r="B140" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C140" s="6" t="s">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="C140" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="D140" s="12" t="s">
-        <v>207</v>
+        <v>69</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -3070,13 +3088,13 @@
         <v>235</v>
       </c>
       <c r="B141" s="11" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C141" s="0" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="C141" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D141" s="12" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -3084,26 +3102,82 @@
         <v>236</v>
       </c>
       <c r="B142" s="11" t="n">
-        <v>0.95</v>
+        <v>3600</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D142" s="12" t="s">
-        <v>211</v>
+        <v>237</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A143" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B143" s="11" t="n">
+        <v>3600</v>
+      </c>
+      <c r="C143" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D143" s="12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A144" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B144" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C143" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D143" s="12" t="s">
+      <c r="C144" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D144" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A145" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B145" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C145" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D145" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A146" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B146" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C146" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D146" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A147" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B147" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D147" s="12" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3113,11 +3187,11 @@
       <formula1>"False,True"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B45:B46 B61:B62 B73:B74 B85:B86 B104:B105 B125:B126 B128" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B45:B46 B61:B62 B73:B74 B85:B86 B104:B105 B127:B128 B130" type="list">
       <formula1>"True,False,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B32 B110 B131" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B32 B110 B133" type="list">
       <formula1>"False,True,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3129,7 +3203,7 @@
       <formula1>"AC,DC"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B64 B76 B88 B108 B129" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B64 B76 B88 B108 B131" type="list">
       <formula1>"AC,DC,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3157,10 +3231,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E144"/>
+  <dimension ref="A1:E148"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A140" activeCellId="0" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -3211,7 +3285,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>35</v>
@@ -3364,7 +3438,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B19" s="8" t="n">
         <v>10000000</v>
@@ -4607,55 +4681,55 @@
         <v>200</v>
       </c>
       <c r="B116" s="11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>69</v>
+        <v>201</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A117" s="10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B117" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C117" s="6" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B118" s="11" t="n">
-        <v>11000</v>
+        <v>10</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>203</v>
+        <v>69</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A119" s="10" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B119" s="11" t="n">
-        <v>11000</v>
-      </c>
-      <c r="C119" s="0" t="s">
-        <v>56</v>
+        <v>0.5</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D119" s="12" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -4663,10 +4737,10 @@
         <v>206</v>
       </c>
       <c r="B120" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C120" s="6" t="s">
-        <v>28</v>
+        <v>11000</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D120" s="12" t="s">
         <v>207</v>
@@ -4677,10 +4751,10 @@
         <v>208</v>
       </c>
       <c r="B121" s="11" t="n">
-        <v>0.95</v>
+        <v>11000</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D121" s="12" t="s">
         <v>209</v>
@@ -4691,9 +4765,9 @@
         <v>210</v>
       </c>
       <c r="B122" s="11" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C122" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C122" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D122" s="12" t="s">
@@ -4705,232 +4779,232 @@
         <v>212</v>
       </c>
       <c r="B123" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D123" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A124" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B124" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D124" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A125" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B125" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C123" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D123" s="12" t="s">
+      <c r="C125" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D125" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="125" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="3"/>
-    </row>
-    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A126" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B126" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C126" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D126" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A127" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B127" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C127" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D127" s="12" t="s">
-        <v>87</v>
-      </c>
+    <row r="127" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B127" s="2"/>
+      <c r="C127" s="2"/>
+      <c r="D127" s="3"/>
     </row>
     <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B128" s="8" t="n">
-        <v>30000</v>
+        <v>218</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>156</v>
+        <v>54</v>
       </c>
       <c r="D128" s="12" t="s">
-        <v>217</v>
+        <v>76</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A129" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="B129" s="6" t="s">
-        <v>186</v>
+        <v>219</v>
+      </c>
+      <c r="B129" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
       <c r="D129" s="12" t="s">
-        <v>184</v>
+        <v>87</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A130" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="B130" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C130" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D130" s="21" t="s">
-        <v>80</v>
+      <c r="A130" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B130" s="8" t="n">
+        <v>30000</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D130" s="12" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A131" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="B131" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>186</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>28</v>
+        <v>187</v>
       </c>
       <c r="D131" s="12" t="s">
-        <v>222</v>
+        <v>184</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A132" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="B132" s="19" t="n">
-        <v>0</v>
+      <c r="B132" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="C132" s="20" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="D132" s="21" t="s">
-        <v>194</v>
+        <v>80</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A133" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="B133" s="11" t="n">
-        <v>10</v>
+      <c r="B133" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="C133" s="0" t="s">
         <v>28</v>
       </c>
       <c r="D133" s="12" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A134" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="B134" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C134" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D134" s="12" t="s">
-        <v>61</v>
+      <c r="A134" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B134" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C134" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D134" s="21" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A135" s="10" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B135" s="11" t="n">
-        <f aca="false">0.03*B134</f>
-        <v>0.015</v>
+        <v>10</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>162</v>
+        <v>28</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>64</v>
+        <v>196</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A136" s="10" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B136" s="11" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C136" s="0" t="s">
         <v>66</v>
       </c>
       <c r="D136" s="12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A137" s="10" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B137" s="11" t="n">
-        <v>10</v>
+        <f aca="false">0.03*B136</f>
+        <v>0.015</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>48</v>
+        <v>162</v>
       </c>
       <c r="D137" s="12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A138" s="10" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B138" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C138" s="6" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="C138" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="D138" s="12" t="s">
-        <v>175</v>
+        <v>67</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A139" s="10" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B139" s="11" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D139" s="12" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A140" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B140" s="11" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D140" s="12" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -4938,13 +5012,13 @@
         <v>234</v>
       </c>
       <c r="B141" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C141" s="6" t="s">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="C141" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="D141" s="12" t="s">
-        <v>207</v>
+        <v>69</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -4952,13 +5026,13 @@
         <v>235</v>
       </c>
       <c r="B142" s="11" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C142" s="0" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="C142" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D142" s="12" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -4966,26 +5040,82 @@
         <v>236</v>
       </c>
       <c r="B143" s="11" t="n">
-        <v>0.95</v>
+        <v>3600</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D143" s="12" t="s">
-        <v>211</v>
+        <v>237</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A144" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B144" s="11" t="n">
+        <v>3600</v>
+      </c>
+      <c r="C144" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D144" s="12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A145" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B145" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C144" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D144" s="12" t="s">
+      <c r="C145" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D145" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A146" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B146" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C146" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D146" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A147" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B147" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D147" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A148" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B148" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C148" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D148" s="12" t="s">
         <v>71</v>
       </c>
     </row>
@@ -5003,7 +5133,7 @@
       <formula1>"uc,tc,cc,v2v,v2g"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B65 B77 B89 B109 B130" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B65 B77 B89 B109 B132" type="list">
       <formula1>"AC,DC,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5011,11 +5141,11 @@
       <formula1>"AC,DC"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B33 B111 B132" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B33 B111 B134" type="list">
       <formula1>"False,True,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B46:B47 B62:B63 B74:B75 B86:B87 B105:B106 B126:B127 B129" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B46:B47 B62:B63 B74:B75 B86:B87 B105:B106 B128:B129 B131" type="list">
       <formula1>"True,False,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5039,10 +5169,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E143"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A139" activeCellId="0" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -6475,55 +6605,55 @@
         <v>200</v>
       </c>
       <c r="B115" s="11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>69</v>
+        <v>201</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B116" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A117" s="10" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B117" s="11" t="n">
-        <v>11000</v>
+        <v>10</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>203</v>
+        <v>69</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B118" s="11" t="n">
-        <v>11000</v>
-      </c>
-      <c r="C118" s="0" t="s">
-        <v>56</v>
+        <v>0.5</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -6531,10 +6661,10 @@
         <v>206</v>
       </c>
       <c r="B119" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>28</v>
+        <v>11000</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D119" s="12" t="s">
         <v>207</v>
@@ -6545,10 +6675,10 @@
         <v>208</v>
       </c>
       <c r="B120" s="11" t="n">
-        <v>0.95</v>
+        <v>11000</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D120" s="12" t="s">
         <v>209</v>
@@ -6559,9 +6689,9 @@
         <v>210</v>
       </c>
       <c r="B121" s="11" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C121" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D121" s="12" t="s">
@@ -6573,232 +6703,232 @@
         <v>212</v>
       </c>
       <c r="B122" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D122" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A123" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B123" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D123" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A124" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B124" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C122" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D122" s="12" t="s">
+      <c r="C124" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D124" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="124" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="3"/>
-    </row>
-    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A125" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B125" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C125" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D125" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A126" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B126" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C126" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D126" s="12" t="s">
-        <v>87</v>
-      </c>
+    <row r="126" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
+      <c r="D126" s="3"/>
     </row>
     <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B127" s="8" t="n">
-        <v>30000</v>
+        <v>218</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>156</v>
+        <v>54</v>
       </c>
       <c r="D127" s="12" t="s">
-        <v>217</v>
+        <v>76</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>186</v>
+        <v>219</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
       <c r="D128" s="12" t="s">
-        <v>184</v>
+        <v>87</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A129" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="B129" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C129" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D129" s="21" t="s">
-        <v>80</v>
+      <c r="A129" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B129" s="8" t="n">
+        <v>30000</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D129" s="12" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A130" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="B130" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>186</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>28</v>
+        <v>187</v>
       </c>
       <c r="D130" s="12" t="s">
-        <v>222</v>
+        <v>184</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A131" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="B131" s="19" t="n">
-        <v>0</v>
+      <c r="B131" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="D131" s="21" t="s">
-        <v>194</v>
+        <v>80</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A132" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="B132" s="11" t="n">
-        <v>10</v>
+      <c r="B132" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="C132" s="0" t="s">
         <v>28</v>
       </c>
       <c r="D132" s="12" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A133" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="B133" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C133" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D133" s="12" t="s">
-        <v>61</v>
+      <c r="A133" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B133" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C133" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D133" s="21" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A134" s="10" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B134" s="11" t="n">
-        <f aca="false">0.03*B133</f>
-        <v>0.015</v>
+        <v>10</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>162</v>
+        <v>28</v>
       </c>
       <c r="D134" s="12" t="s">
-        <v>64</v>
+        <v>196</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A135" s="10" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B135" s="11" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C135" s="0" t="s">
         <v>66</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A136" s="10" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B136" s="11" t="n">
-        <v>10</v>
+        <f aca="false">0.03*B135</f>
+        <v>0.015</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>48</v>
+        <v>162</v>
       </c>
       <c r="D136" s="12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A137" s="10" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B137" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C137" s="6" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="C137" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="D137" s="12" t="s">
-        <v>175</v>
+        <v>67</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A138" s="10" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B138" s="11" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D138" s="12" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A139" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B139" s="11" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D139" s="12" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -6806,13 +6936,13 @@
         <v>234</v>
       </c>
       <c r="B140" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C140" s="6" t="s">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="C140" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="D140" s="12" t="s">
-        <v>207</v>
+        <v>69</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -6820,13 +6950,13 @@
         <v>235</v>
       </c>
       <c r="B141" s="11" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C141" s="0" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="C141" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D141" s="12" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -6834,26 +6964,82 @@
         <v>236</v>
       </c>
       <c r="B142" s="11" t="n">
-        <v>0.95</v>
+        <v>3600</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D142" s="12" t="s">
-        <v>211</v>
+        <v>237</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A143" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B143" s="11" t="n">
+        <v>3600</v>
+      </c>
+      <c r="C143" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D143" s="12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A144" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B144" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C143" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D143" s="12" t="s">
+      <c r="C144" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D144" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A145" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B145" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C145" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D145" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A146" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B146" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C146" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D146" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A147" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B147" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D147" s="12" t="s">
         <v>71</v>
       </c>
     </row>
@@ -6863,11 +7049,11 @@
       <formula1>"False,True"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B45:B46 B61:B62 B73:B74 B85:B86 B104:B105 B125:B126 B128" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B45:B46 B61:B62 B73:B74 B85:B86 B104:B105 B127:B128 B130" type="list">
       <formula1>"True,False,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B32 B110 B131" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B32 B110 B133" type="list">
       <formula1>"False,True,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6879,7 +7065,7 @@
       <formula1>"AC,DC"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B64 B76 B88 B108 B129" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B64 B76 B88 B108 B131" type="list">
       <formula1>"AC,DC,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6907,10 +7093,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E143"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A139" activeCellId="0" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -8323,7 +8509,7 @@
     </row>
     <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A114" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B114" s="11" t="n">
         <v>0</v>
@@ -8332,63 +8518,63 @@
         <v>66</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>67</v>
+        <v>201</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A115" s="10" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B115" s="11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>69</v>
+        <v>203</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B116" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>175</v>
+        <v>67</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A117" s="10" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B117" s="11" t="n">
-        <v>11000</v>
+        <v>10</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>203</v>
+        <v>69</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B118" s="11" t="n">
-        <v>11000</v>
-      </c>
-      <c r="C118" s="0" t="s">
-        <v>56</v>
+        <v>0.5</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -8396,10 +8582,10 @@
         <v>206</v>
       </c>
       <c r="B119" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>28</v>
+        <v>11000</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D119" s="12" t="s">
         <v>207</v>
@@ -8410,10 +8596,10 @@
         <v>208</v>
       </c>
       <c r="B120" s="11" t="n">
-        <v>0.95</v>
+        <v>11000</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D120" s="12" t="s">
         <v>209</v>
@@ -8424,9 +8610,9 @@
         <v>210</v>
       </c>
       <c r="B121" s="11" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C121" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D121" s="12" t="s">
@@ -8438,232 +8624,232 @@
         <v>212</v>
       </c>
       <c r="B122" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D122" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A123" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B123" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D123" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A124" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B124" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C122" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D122" s="12" t="s">
+      <c r="C124" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D124" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="124" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="3"/>
-    </row>
-    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A125" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B125" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C125" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D125" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A126" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B126" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C126" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D126" s="12" t="s">
-        <v>87</v>
-      </c>
+    <row r="126" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
+      <c r="D126" s="3"/>
     </row>
     <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B127" s="8" t="n">
-        <v>30000</v>
+        <v>218</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>156</v>
+        <v>54</v>
       </c>
       <c r="D127" s="12" t="s">
-        <v>217</v>
+        <v>76</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>186</v>
+        <v>219</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
       <c r="D128" s="12" t="s">
-        <v>184</v>
+        <v>87</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A129" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="B129" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C129" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D129" s="21" t="s">
-        <v>80</v>
+      <c r="A129" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B129" s="8" t="n">
+        <v>30000</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D129" s="12" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A130" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="B130" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>186</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>28</v>
+        <v>187</v>
       </c>
       <c r="D130" s="12" t="s">
-        <v>222</v>
+        <v>184</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A131" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="B131" s="19" t="n">
-        <v>0</v>
+      <c r="B131" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="D131" s="21" t="s">
-        <v>194</v>
+        <v>80</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A132" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="B132" s="11" t="n">
-        <v>10</v>
+      <c r="B132" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="C132" s="0" t="s">
         <v>28</v>
       </c>
       <c r="D132" s="12" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A133" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="B133" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C133" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D133" s="12" t="s">
-        <v>61</v>
+      <c r="A133" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B133" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C133" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D133" s="21" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A134" s="10" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B134" s="11" t="n">
-        <f aca="false">0.03*B133</f>
-        <v>0.015</v>
+        <v>10</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>162</v>
+        <v>28</v>
       </c>
       <c r="D134" s="12" t="s">
-        <v>64</v>
+        <v>196</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A135" s="10" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B135" s="11" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C135" s="0" t="s">
         <v>66</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A136" s="10" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B136" s="11" t="n">
-        <v>10</v>
+        <f aca="false">0.03*B135</f>
+        <v>0.015</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>48</v>
+        <v>162</v>
       </c>
       <c r="D136" s="12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A137" s="10" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B137" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C137" s="6" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="C137" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="D137" s="12" t="s">
-        <v>175</v>
+        <v>67</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A138" s="10" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B138" s="11" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D138" s="12" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A139" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B139" s="11" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D139" s="12" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -8671,13 +8857,13 @@
         <v>234</v>
       </c>
       <c r="B140" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C140" s="6" t="s">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="C140" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="D140" s="12" t="s">
-        <v>207</v>
+        <v>69</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -8685,13 +8871,13 @@
         <v>235</v>
       </c>
       <c r="B141" s="11" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C141" s="0" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="C141" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D141" s="12" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -8699,26 +8885,82 @@
         <v>236</v>
       </c>
       <c r="B142" s="11" t="n">
-        <v>0.95</v>
+        <v>3600</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D142" s="12" t="s">
-        <v>211</v>
+        <v>237</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A143" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B143" s="11" t="n">
+        <v>3600</v>
+      </c>
+      <c r="C143" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D143" s="12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A144" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B144" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C143" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D143" s="12" t="s">
+      <c r="C144" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D144" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A145" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B145" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C145" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D145" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A146" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B146" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C146" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D146" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A147" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B147" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D147" s="12" t="s">
         <v>71</v>
       </c>
     </row>
@@ -8728,11 +8970,11 @@
       <formula1>"False,True"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B45:B46 B61:B62 B73:B74 B85:B86 B104:B105 B125:B126 B128" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B45:B46 B61:B62 B73:B74 B85:B86 B104:B105 B127:B128 B130" type="list">
       <formula1>"True,False,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B32 B110 B131" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B32 B110 B133" type="list">
       <formula1>"False,True,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8744,7 +8986,7 @@
       <formula1>"AC,DC"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B64 B76 B88 B108 B129" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B64 B76 B88 B108 B131" type="list">
       <formula1>"AC,DC,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8772,10 +9014,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E143"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A139" activeCellId="0" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -8826,7 +9068,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>35</v>
@@ -10205,55 +10447,55 @@
         <v>200</v>
       </c>
       <c r="B115" s="11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>69</v>
+        <v>201</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B116" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A117" s="10" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B117" s="11" t="n">
-        <v>11000</v>
+        <v>10</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>203</v>
+        <v>69</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B118" s="11" t="n">
-        <v>11000</v>
-      </c>
-      <c r="C118" s="0" t="s">
-        <v>56</v>
+        <v>0.5</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -10261,10 +10503,10 @@
         <v>206</v>
       </c>
       <c r="B119" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>28</v>
+        <v>11000</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D119" s="12" t="s">
         <v>207</v>
@@ -10275,10 +10517,10 @@
         <v>208</v>
       </c>
       <c r="B120" s="11" t="n">
-        <v>0.95</v>
+        <v>11000</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D120" s="12" t="s">
         <v>209</v>
@@ -10289,9 +10531,9 @@
         <v>210</v>
       </c>
       <c r="B121" s="11" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C121" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D121" s="12" t="s">
@@ -10303,232 +10545,232 @@
         <v>212</v>
       </c>
       <c r="B122" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D122" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A123" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B123" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D123" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A124" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B124" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C122" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D122" s="12" t="s">
+      <c r="C124" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D124" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="124" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="3"/>
-    </row>
-    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A125" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B125" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C125" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D125" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A126" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B126" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C126" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D126" s="12" t="s">
-        <v>87</v>
-      </c>
+    <row r="126" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
+      <c r="D126" s="3"/>
     </row>
     <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B127" s="8" t="n">
-        <v>30000</v>
+        <v>218</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>156</v>
+        <v>54</v>
       </c>
       <c r="D127" s="12" t="s">
-        <v>217</v>
+        <v>76</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>186</v>
+        <v>219</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
       <c r="D128" s="12" t="s">
-        <v>184</v>
+        <v>87</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A129" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="B129" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C129" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D129" s="21" t="s">
-        <v>80</v>
+      <c r="A129" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B129" s="8" t="n">
+        <v>30000</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D129" s="12" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A130" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="B130" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>186</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>28</v>
+        <v>187</v>
       </c>
       <c r="D130" s="12" t="s">
-        <v>222</v>
+        <v>184</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A131" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="B131" s="19" t="n">
-        <v>0</v>
+      <c r="B131" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="D131" s="21" t="s">
-        <v>194</v>
+        <v>80</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A132" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="B132" s="11" t="n">
-        <v>10</v>
+      <c r="B132" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="C132" s="0" t="s">
         <v>28</v>
       </c>
       <c r="D132" s="12" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A133" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="B133" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C133" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D133" s="12" t="s">
-        <v>61</v>
+      <c r="A133" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B133" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C133" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D133" s="21" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A134" s="10" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B134" s="11" t="n">
-        <f aca="false">0.03*B133</f>
-        <v>0.015</v>
+        <v>10</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>162</v>
+        <v>28</v>
       </c>
       <c r="D134" s="12" t="s">
-        <v>64</v>
+        <v>196</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A135" s="10" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B135" s="11" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C135" s="0" t="s">
         <v>66</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A136" s="10" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B136" s="11" t="n">
-        <v>10</v>
+        <f aca="false">0.03*B135</f>
+        <v>0.015</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>48</v>
+        <v>162</v>
       </c>
       <c r="D136" s="12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A137" s="10" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B137" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C137" s="6" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="C137" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="D137" s="12" t="s">
-        <v>175</v>
+        <v>67</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A138" s="10" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B138" s="11" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D138" s="12" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A139" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B139" s="11" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D139" s="12" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -10536,13 +10778,13 @@
         <v>234</v>
       </c>
       <c r="B140" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C140" s="6" t="s">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="C140" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="D140" s="12" t="s">
-        <v>207</v>
+        <v>69</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -10550,13 +10792,13 @@
         <v>235</v>
       </c>
       <c r="B141" s="11" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C141" s="0" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="C141" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D141" s="12" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -10564,26 +10806,82 @@
         <v>236</v>
       </c>
       <c r="B142" s="11" t="n">
-        <v>0.95</v>
+        <v>3600</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D142" s="12" t="s">
-        <v>211</v>
+        <v>237</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A143" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B143" s="11" t="n">
+        <v>3600</v>
+      </c>
+      <c r="C143" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D143" s="12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A144" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B144" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C143" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D143" s="12" t="s">
+      <c r="C144" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D144" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A145" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B145" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C145" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D145" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A146" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B146" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C146" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D146" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A147" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B147" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D147" s="12" t="s">
         <v>71</v>
       </c>
     </row>
@@ -10593,11 +10891,11 @@
       <formula1>"False,True"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B45:B46 B61:B62 B73:B74 B85:B86 B104:B105 B125:B126 B128" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B45:B46 B61:B62 B73:B74 B85:B86 B104:B105 B127:B128 B130" type="list">
       <formula1>"True,False,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B32 B110 B131" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B32 B110 B133" type="list">
       <formula1>"False,True,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -10609,7 +10907,7 @@
       <formula1>"AC,DC"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B64 B76 B88 B108 B129" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B64 B76 B88 B108 B131" type="list">
       <formula1>"AC,DC,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -10637,10 +10935,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E143"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B151" activeCellId="0" sqref="B151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -12070,55 +12368,55 @@
         <v>200</v>
       </c>
       <c r="B115" s="11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>69</v>
+        <v>201</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B116" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A117" s="10" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B117" s="11" t="n">
-        <v>11000</v>
+        <v>10</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>203</v>
+        <v>69</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B118" s="11" t="n">
-        <v>11000</v>
-      </c>
-      <c r="C118" s="0" t="s">
-        <v>56</v>
+        <v>0.5</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -12126,10 +12424,10 @@
         <v>206</v>
       </c>
       <c r="B119" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>28</v>
+        <v>11000</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="D119" s="12" t="s">
         <v>207</v>
@@ -12140,10 +12438,10 @@
         <v>208</v>
       </c>
       <c r="B120" s="11" t="n">
-        <v>0.95</v>
+        <v>11000</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D120" s="12" t="s">
         <v>209</v>
@@ -12154,9 +12452,9 @@
         <v>210</v>
       </c>
       <c r="B121" s="11" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C121" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D121" s="12" t="s">
@@ -12168,232 +12466,232 @@
         <v>212</v>
       </c>
       <c r="B122" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D122" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A123" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B123" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D123" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A124" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B124" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C122" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D122" s="12" t="s">
+      <c r="C124" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D124" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="124" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="3"/>
-    </row>
-    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A125" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B125" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C125" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D125" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A126" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B126" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C126" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D126" s="12" t="s">
-        <v>87</v>
-      </c>
+    <row r="126" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
+      <c r="D126" s="3"/>
     </row>
     <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B127" s="8" t="n">
-        <v>30000</v>
+        <v>218</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>156</v>
+        <v>54</v>
       </c>
       <c r="D127" s="12" t="s">
-        <v>217</v>
+        <v>76</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>186</v>
+        <v>219</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
       <c r="D128" s="12" t="s">
-        <v>184</v>
+        <v>87</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A129" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="B129" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C129" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D129" s="21" t="s">
-        <v>80</v>
+      <c r="A129" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B129" s="8" t="n">
+        <v>30000</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D129" s="12" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A130" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="B130" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>186</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>28</v>
+        <v>187</v>
       </c>
       <c r="D130" s="12" t="s">
-        <v>222</v>
+        <v>184</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A131" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="B131" s="19" t="n">
-        <v>0</v>
+      <c r="B131" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="D131" s="21" t="s">
-        <v>194</v>
+        <v>80</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A132" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="B132" s="11" t="n">
-        <v>10</v>
+      <c r="B132" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="C132" s="0" t="s">
         <v>28</v>
       </c>
       <c r="D132" s="12" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A133" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="B133" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C133" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D133" s="12" t="s">
-        <v>61</v>
+      <c r="A133" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B133" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C133" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D133" s="21" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A134" s="10" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B134" s="11" t="n">
-        <f aca="false">0.03*B133</f>
-        <v>0.015</v>
+        <v>10</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>162</v>
+        <v>28</v>
       </c>
       <c r="D134" s="12" t="s">
-        <v>64</v>
+        <v>196</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A135" s="10" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B135" s="11" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C135" s="0" t="s">
         <v>66</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A136" s="10" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B136" s="11" t="n">
-        <v>10</v>
+        <f aca="false">0.03*B135</f>
+        <v>0.015</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>48</v>
+        <v>162</v>
       </c>
       <c r="D136" s="12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A137" s="10" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B137" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C137" s="6" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="C137" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="D137" s="12" t="s">
-        <v>175</v>
+        <v>67</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A138" s="10" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B138" s="11" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D138" s="12" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A139" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B139" s="11" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D139" s="12" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -12401,13 +12699,13 @@
         <v>234</v>
       </c>
       <c r="B140" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C140" s="6" t="s">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="C140" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="D140" s="12" t="s">
-        <v>207</v>
+        <v>69</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -12415,13 +12713,13 @@
         <v>235</v>
       </c>
       <c r="B141" s="11" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C141" s="0" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="C141" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D141" s="12" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -12429,26 +12727,82 @@
         <v>236</v>
       </c>
       <c r="B142" s="11" t="n">
-        <v>0.95</v>
+        <v>3600</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D142" s="12" t="s">
-        <v>211</v>
+        <v>237</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A143" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B143" s="11" t="n">
+        <v>3600</v>
+      </c>
+      <c r="C143" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D143" s="12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A144" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B144" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C143" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D143" s="12" t="s">
+      <c r="C144" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D144" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A145" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B145" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C145" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D145" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A146" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B146" s="11" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C146" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D146" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A147" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B147" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D147" s="12" t="s">
         <v>71</v>
       </c>
     </row>
@@ -12458,11 +12812,11 @@
       <formula1>"False,True"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B45:B46 B61:B62 B73:B74 B85:B86 B104:B105 B125:B126 B128" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B45:B46 B61:B62 B73:B74 B85:B86 B104:B105 B127:B128 B130" type="list">
       <formula1>"True,False,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B32 B110 B131" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B32 B110 B133" type="list">
       <formula1>"False,True,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -12474,7 +12828,7 @@
       <formula1>"AC,DC"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B64 B76 B88 B108 B129" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B64 B76 B88 B108 B131" type="list">
       <formula1>"AC,DC,"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>